<commit_message>
chore: update test runner and frontend config
</commit_message>
<xml_diff>
--- a/backend/src/templates/testcase_template.xlsx
+++ b/backend/src/templates/testcase_template.xlsx
@@ -398,7 +398,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -407,7 +407,8 @@
     <col min="2" max="2" width="30.83203125" customWidth="1"/>
     <col min="3" max="3" width="35.83203125" customWidth="1"/>
     <col min="4" max="4" width="12.83203125" customWidth="1"/>
-    <col min="5" max="5" width="50.83203125" customWidth="1"/>
+    <col min="5" max="5" width="14.83203125" customWidth="1"/>
+    <col min="6" max="6" width="50.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -424,6 +425,9 @@
         <v>trinh_duyet</v>
       </c>
       <c r="E1" t="str">
+        <v>thiet_bi</v>
+      </c>
+      <c r="F1" t="str">
         <v>buoc_thuc_hien</v>
       </c>
     </row>
@@ -441,6 +445,9 @@
         <v>chromium</v>
       </c>
       <c r="E2" t="str">
+        <v/>
+      </c>
+      <c r="F2" t="str">
         <v>Mở trang https://example.com/login</v>
       </c>
     </row>
@@ -458,6 +465,9 @@
         <v/>
       </c>
       <c r="E3" t="str">
+        <v/>
+      </c>
+      <c r="F3" t="str">
         <v>Nhập "user@test.com" vào ô Email</v>
       </c>
     </row>
@@ -475,6 +485,9 @@
         <v/>
       </c>
       <c r="E4" t="str">
+        <v/>
+      </c>
+      <c r="F4" t="str">
         <v>Nhập "password123" vào ô Mật khẩu</v>
       </c>
     </row>
@@ -492,6 +505,9 @@
         <v/>
       </c>
       <c r="E5" t="str">
+        <v/>
+      </c>
+      <c r="F5" t="str">
         <v>Nhấn nút "Đăng nhập"</v>
       </c>
     </row>
@@ -509,6 +525,9 @@
         <v/>
       </c>
       <c r="E6" t="str">
+        <v/>
+      </c>
+      <c r="F6" t="str">
         <v>Kiểm tra URL chứa /dashboard</v>
       </c>
     </row>
@@ -526,6 +545,9 @@
         <v/>
       </c>
       <c r="E7" t="str">
+        <v/>
+      </c>
+      <c r="F7" t="str">
         <v>Chụp ảnh màn hình</v>
       </c>
     </row>
@@ -534,15 +556,18 @@
         <v>TC-002</v>
       </c>
       <c r="B8" t="str">
-        <v>Kiểm tra trang chủ</v>
+        <v>Kiểm tra trang chủ (Mobile)</v>
       </c>
       <c r="C8" t="str">
         <v>https://example.com</v>
       </c>
       <c r="D8" t="str">
-        <v>chromium</v>
+        <v>webkit</v>
       </c>
       <c r="E8" t="str">
+        <v>iphone-15</v>
+      </c>
+      <c r="F8" t="str">
         <v>Mở trang https://example.com</v>
       </c>
     </row>
@@ -560,6 +585,9 @@
         <v/>
       </c>
       <c r="E9" t="str">
+        <v/>
+      </c>
+      <c r="F9" t="str">
         <v>Kiểm tra phần tử h1 hiển thị</v>
       </c>
     </row>
@@ -577,6 +605,9 @@
         <v/>
       </c>
       <c r="E10" t="str">
+        <v/>
+      </c>
+      <c r="F10" t="str">
         <v>Chờ 2 giây</v>
       </c>
     </row>
@@ -594,19 +625,22 @@
         <v/>
       </c>
       <c r="E11" t="str">
+        <v/>
+      </c>
+      <c r="F11" t="str">
         <v>Chụp ảnh màn hình</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:E11"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F11"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C28"/>
+  <dimension ref="A1:C45"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -683,190 +717,365 @@
     </row>
     <row r="8">
       <c r="A8" t="str">
-        <v>buoc_thuc_hien</v>
+        <v>thiet_bi</v>
       </c>
       <c r="B8" t="str">
-        <v>Mô tả bước bằng ngôn ngữ tự nhiên</v>
+        <v>Thiết bị mobile (xem danh sách bên dưới). Để trống = Desktop</v>
       </c>
       <c r="C8" t="str">
-        <v>Có</v>
+        <v>Không</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="str">
-        <v/>
+        <v>buoc_thuc_hien</v>
+      </c>
+      <c r="B9" t="str">
+        <v>Mô tả bước bằng ngôn ngữ tự nhiên</v>
+      </c>
+      <c r="C9" t="str">
+        <v>Có</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="str">
-        <v>CÁC MẪU CÂU HỖ TRỢ:</v>
+        <v/>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="str">
-        <v>Hành động</v>
-      </c>
-      <c r="B11" t="str">
-        <v>Cách viết</v>
-      </c>
-      <c r="C11" t="str">
-        <v>Ví dụ</v>
+        <v>CÁC MẪU CÂU HỖ TRỢ:</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="str">
-        <v>Mở trang</v>
+        <v>Hành động</v>
       </c>
       <c r="B12" t="str">
-        <v>Mở trang &lt;URL&gt;</v>
+        <v>Cách viết</v>
       </c>
       <c r="C12" t="str">
-        <v>Mở trang https://example.com</v>
+        <v>Ví dụ</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="str">
-        <v>Nhập liệu</v>
+        <v>Mở trang</v>
       </c>
       <c r="B13" t="str">
-        <v>Nhập "&lt;giá trị&gt;" vào ô &lt;tên trường&gt;</v>
+        <v>Mở trang &lt;URL&gt;</v>
       </c>
       <c r="C13" t="str">
-        <v>Nhập "admin" vào ô Email</v>
+        <v>Mở trang https://example.com</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="str">
-        <v>Nhấn nút</v>
+        <v>Nhập liệu</v>
       </c>
       <c r="B14" t="str">
-        <v>Nhấn nút "&lt;tên nút&gt;"</v>
+        <v>Nhập "&lt;giá trị&gt;" vào ô &lt;tên trường&gt;</v>
       </c>
       <c r="C14" t="str">
-        <v>Nhấn nút "Đăng nhập"</v>
+        <v>Nhập "admin" vào ô Email</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="str">
-        <v>Click link</v>
+        <v>Nhấn nút</v>
       </c>
       <c r="B15" t="str">
-        <v>Click vào link "&lt;text&gt;"</v>
+        <v>Nhấn nút "&lt;tên nút&gt;"</v>
       </c>
       <c r="C15" t="str">
-        <v>Click vào link "Quên mật khẩu"</v>
+        <v>Nhấn nút "Đăng nhập"</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="str">
-        <v>Chọn dropdown</v>
+        <v>Click link</v>
       </c>
       <c r="B16" t="str">
-        <v>Chọn "&lt;giá trị&gt;" trong dropdown &lt;tên&gt;</v>
+        <v>Click vào link "&lt;text&gt;"</v>
       </c>
       <c r="C16" t="str">
-        <v>Chọn "VN" trong dropdown Quốc gia</v>
+        <v>Click vào link "Quên mật khẩu"</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="str">
-        <v>Kiểm tra text</v>
+        <v>Chọn dropdown</v>
       </c>
       <c r="B17" t="str">
-        <v>Kiểm tra text "&lt;text&gt;" hiển thị</v>
+        <v>Chọn "&lt;giá trị&gt;" trong dropdown &lt;tên&gt;</v>
       </c>
       <c r="C17" t="str">
-        <v>Kiểm tra text "Xin chào" hiển thị</v>
+        <v>Chọn "VN" trong dropdown Quốc gia</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="str">
-        <v>Kiểm tra URL</v>
+        <v>Kiểm tra text</v>
       </c>
       <c r="B18" t="str">
-        <v>Kiểm tra URL chứa &lt;path&gt;</v>
+        <v>Kiểm tra text "&lt;text&gt;" hiển thị</v>
       </c>
       <c r="C18" t="str">
-        <v>Kiểm tra URL chứa /dashboard</v>
+        <v>Kiểm tra text "Xin chào" hiển thị</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="str">
-        <v>Kiểm tra hiển thị</v>
+        <v>Kiểm tra URL</v>
       </c>
       <c r="B19" t="str">
-        <v>Kiểm tra phần tử &lt;selector&gt; hiển thị</v>
+        <v>Kiểm tra URL chứa &lt;path&gt;</v>
       </c>
       <c r="C19" t="str">
-        <v>Kiểm tra phần tử #header hiển thị</v>
+        <v>Kiểm tra URL chứa /dashboard</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="str">
-        <v>Chờ</v>
+        <v>Kiểm tra hiển thị</v>
       </c>
       <c r="B20" t="str">
-        <v>Chờ &lt;N&gt; giây</v>
+        <v>Kiểm tra phần tử &lt;selector&gt; hiển thị</v>
       </c>
       <c r="C20" t="str">
-        <v>Chờ 3 giây</v>
+        <v>Kiểm tra phần tử #header hiển thị</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="str">
-        <v>Chụp ảnh</v>
+        <v>Chờ</v>
       </c>
       <c r="B21" t="str">
-        <v>Chụp ảnh màn hình</v>
+        <v>Chờ &lt;N&gt; giây</v>
       </c>
       <c r="C21" t="str">
-        <v>Chụp ảnh màn hình</v>
+        <v>Chờ 3 giây</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="str">
-        <v>Di chuột</v>
+        <v>Chụp ảnh</v>
       </c>
       <c r="B22" t="str">
-        <v>Di chuột vào &lt;phần tử&gt;</v>
+        <v>Chụp ảnh màn hình</v>
       </c>
       <c r="C22" t="str">
-        <v>Di chuột vào menu "Sản phẩm"</v>
+        <v>Chụp ảnh màn hình</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="str">
-        <v/>
+        <v>Di chuột</v>
+      </c>
+      <c r="B23" t="str">
+        <v>Di chuột vào &lt;phần tử&gt;</v>
+      </c>
+      <c r="C23" t="str">
+        <v>Di chuột vào menu "Sản phẩm"</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="str">
-        <v>LƯU Ý:</v>
+        <v/>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="str">
-        <v>- Mỗi dòng = 1 bước thực hiện</v>
+        <v>LƯU Ý:</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="str">
-        <v>- Các dòng cùng tc_id thuộc cùng 1 test case</v>
+        <v>- Mỗi dòng = 1 bước thực hiện</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="str">
-        <v>- Cột tieu_de, url, trinh_duyet chỉ cần ghi ở dòng đầu tiên của mỗi test case</v>
+        <v>- Các dòng cùng tc_id thuộc cùng 1 test case</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="str">
+        <v>- Cột tieu_de, url, trinh_duyet, thiet_bi chỉ cần ghi ở dòng đầu tiên của mỗi test case</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="str">
         <v>- Nếu biết CSS selector, có thể dùng trực tiếp: Nhấn vào #submit-btn</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="str">
+        <v>GIÁ TRỊ HỢP LỆ cho cột thiet_bi:</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="str">
+        <v/>
+      </c>
+      <c r="B32" t="str">
+        <v>iphone-15</v>
+      </c>
+      <c r="C32" t="str">
+        <v>iPhone 15 (390×844)</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="str">
+        <v/>
+      </c>
+      <c r="B33" t="str">
+        <v>iphone-15-pro</v>
+      </c>
+      <c r="C33" t="str">
+        <v>iPhone 15 Pro (393×852)</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="str">
+        <v/>
+      </c>
+      <c r="B34" t="str">
+        <v>iphone-14</v>
+      </c>
+      <c r="C34" t="str">
+        <v>iPhone 14 (390×844)</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="str">
+        <v/>
+      </c>
+      <c r="B35" t="str">
+        <v>iphone-13</v>
+      </c>
+      <c r="C35" t="str">
+        <v>iPhone 13 (390×844)</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="str">
+        <v/>
+      </c>
+      <c r="B36" t="str">
+        <v>iphone-12</v>
+      </c>
+      <c r="C36" t="str">
+        <v>iPhone 12 (390×844)</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="str">
+        <v/>
+      </c>
+      <c r="B37" t="str">
+        <v>iphone-se</v>
+      </c>
+      <c r="C37" t="str">
+        <v>iPhone SE (375×667)</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="str">
+        <v/>
+      </c>
+      <c r="B38" t="str">
+        <v>pixel-7</v>
+      </c>
+      <c r="C38" t="str">
+        <v>Pixel 7 (412×915)</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="str">
+        <v/>
+      </c>
+      <c r="B39" t="str">
+        <v>pixel-5</v>
+      </c>
+      <c r="C39" t="str">
+        <v>Pixel 5 (393×851)</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="str">
+        <v/>
+      </c>
+      <c r="B40" t="str">
+        <v>galaxy-s24</v>
+      </c>
+      <c r="C40" t="str">
+        <v>Galaxy S24 (360×780)</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="str">
+        <v/>
+      </c>
+      <c r="B41" t="str">
+        <v>galaxy-s9</v>
+      </c>
+      <c r="C41" t="str">
+        <v>Galaxy S9+ (320×658)</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="str">
+        <v/>
+      </c>
+      <c r="B42" t="str">
+        <v>ipad-pro</v>
+      </c>
+      <c r="C42" t="str">
+        <v>iPad Pro 11 (834×1194)</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="str">
+        <v/>
+      </c>
+      <c r="B43" t="str">
+        <v>ipad-mini</v>
+      </c>
+      <c r="C43" t="str">
+        <v>iPad Mini (768×1024)</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="str">
+        <v/>
+      </c>
+      <c r="B44" t="str">
+        <v>galaxy-tab</v>
+      </c>
+      <c r="C44" t="str">
+        <v>Galaxy Tab S4 (712×1138)</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="str">
+        <v/>
+      </c>
+      <c r="B45" t="str">
+        <v>(để trống)</v>
+      </c>
+      <c r="C45" t="str">
+        <v>Desktop 1920×1080 (mặc định)</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C28"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C45"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>